<commit_message>
05 verbeterd, 12-10 ingevoerd
</commit_message>
<xml_diff>
--- a/data/Austerlitz_seizoen_2018-2019.xlsx
+++ b/data/Austerlitz_seizoen_2018-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\src\dartsense\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E407896-7350-41BA-A00C-899631DAA061}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6214E58-16EA-4923-AAFD-64EBFE95AFA0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" tabRatio="766" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" tabRatio="766" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-08-31" sheetId="30" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="2018-09-21" sheetId="33" r:id="rId4"/>
     <sheet name="2018-09-28" sheetId="34" r:id="rId5"/>
     <sheet name="2018-10-05" sheetId="35" r:id="rId6"/>
+    <sheet name="2018-10-12" sheetId="36" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="39">
   <si>
     <t>Baan</t>
   </si>
@@ -138,17 +139,36 @@
   <si>
     <t>bye</t>
   </si>
+  <si>
+    <t>Frans</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Ernie</t>
+  </si>
+  <si>
+    <t>Reyn</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -195,8 +215,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -205,13 +226,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 5" xfId="4" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4284,62 +4306,850 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22855EEE-7E26-4EF4-B787-04456A03E58F}">
   <dimension ref="A1:L37"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354FFAA9-6ED0-4FD3-A851-C0A20C7A67C0}">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -4349,83 +5159,77 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
+      <c r="B4">
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
         <v>2</v>
-      </c>
-      <c r="L5">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -4436,85 +5240,82 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
+      <c r="B8">
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -4522,96 +5323,96 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>2</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="1">
-        <v>2</v>
+      <c r="B13">
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="1">
-        <v>2</v>
+      <c r="B14">
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
-      <c r="B15" s="1">
-        <v>2</v>
+      <c r="B15">
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -4624,14 +5425,14 @@
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="1">
-        <v>2</v>
+      <c r="B16" t="s">
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -4642,39 +5443,39 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -4684,14 +5485,14 @@
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="B19" s="1">
-        <v>2</v>
+      <c r="B19">
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -4702,19 +5503,19 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -4724,80 +5525,83 @@
       <c r="A21">
         <v>6</v>
       </c>
-      <c r="B21" s="1">
-        <v>3</v>
+      <c r="B21">
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" s="1">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>2</v>
-      </c>
-      <c r="K22">
-        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -4805,113 +5609,119 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25" s="1">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>6</v>
-      </c>
-      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>6</v>
-      </c>
-      <c r="B30" s="1">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
@@ -4925,79 +5735,82 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" s="1">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>6</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
       <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="H32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" s="1">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -5005,62 +5818,102 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35" s="1">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>3</v>
-      </c>
-      <c r="B36" s="1">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>6</v>
-      </c>
-      <c r="B37" s="1">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
       </c>
       <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
         <v>18</v>
       </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>